<commit_message>
fixed excel sheet saving
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -1,109 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMS\Desktop\www\Python\Al_Halal_POS\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED50E16B-C1EF-4CE2-9A75-A49E66B3A4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="March" sheetId="1" r:id="rId1"/>
+    <sheet name="March" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Item Name</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Quantity Sold</t>
-  </si>
-  <si>
-    <t>Quantity Left</t>
-  </si>
-  <si>
-    <t>Original Price</t>
-  </si>
-  <si>
-    <t>Sale Price</t>
-  </si>
-  <si>
-    <t>Inventory Quantity</t>
-  </si>
-  <si>
-    <t>Barcode</t>
-  </si>
-  <si>
-    <t>Kurt Ermak</t>
-  </si>
-  <si>
-    <t>Invested</t>
-  </si>
-  <si>
-    <t>Clean Profit</t>
-  </si>
-  <si>
-    <t>Total Profit</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$₩-412]* #,##0.00_-;\-[$₩-412]* #,##0.00_-;_-[$₩-412]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="14"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.3499862666707358"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,38 +76,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -455,217 +454,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col width="11.6640625" customWidth="1" min="1" max="1"/>
+    <col width="25.44140625" customWidth="1" style="7" min="2" max="2"/>
+    <col width="20.88671875" customWidth="1" min="3" max="3"/>
+    <col width="22.6640625" customWidth="1" min="4" max="4"/>
+    <col width="17.44140625" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="18.6640625" customWidth="1" min="7" max="7"/>
+    <col width="15.21875" customWidth="1" min="8" max="8"/>
+    <col width="16.44140625" customWidth="1" min="9" max="9"/>
+    <col width="17.44140625" customWidth="1" min="10" max="10"/>
+    <col width="17.6640625" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Barcode</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Item Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Inventory Quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity Sold</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity Left</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Original Price</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Sale Price</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Total Profit</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Invested</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Clean Profit</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="B2" s="6" t="n">
         <v>4780022250220</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Kurt Ermak</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="E2" s="3" t="n">
         <v>100</v>
       </c>
       <c r="F2" s="3">
         <f>D2-E2</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
+        <v/>
+      </c>
+      <c r="G2" s="4" t="n">
         <v>2500</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="4" t="n">
         <v>3000</v>
       </c>
       <c r="I2" s="4">
         <f>H2*E2</f>
-        <v>300000</v>
+        <v/>
       </c>
       <c r="J2" s="2">
         <f>D2*G2</f>
-        <v>250000</v>
+        <v/>
       </c>
       <c r="K2" s="2">
         <f>I2-J2</f>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="n"/>
+      <c r="E4" s="3" t="n"/>
+      <c r="F4" s="3" t="n"/>
+      <c r="G4" s="3" t="n"/>
+      <c r="H4" s="3" t="n"/>
+      <c r="I4" s="3" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
+      <c r="H5" s="3" t="n"/>
+      <c r="I5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="3" t="n"/>
+      <c r="E6" s="3" t="n"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="3" t="n"/>
+      <c r="I6" s="3" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
+      <c r="I7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="3" t="n"/>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="3" t="n"/>
+      <c r="I8" s="3" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="B9" s="6" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="3" t="n"/>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
+      <c r="H9" s="3" t="n"/>
+      <c r="I9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="B10" s="6" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="3" t="n"/>
+      <c r="E10" s="3" t="n"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
+      <c r="H10" s="3" t="n"/>
+      <c r="I10" s="3" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="3" t="n"/>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="3" t="n"/>
+      <c r="I11" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
improved autofocus on barcode inputs
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>100</v>
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>

</xml_diff>

<commit_message>
little improvement of inventory tab
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMS\Desktop\www\Python\Al_Halal_POS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7E2C2-2C71-4D6C-ABEC-0DF60E9835DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B1A0A9-B5C0-4546-BA63-62117CEF0D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>No</t>
   </si>
@@ -68,7 +68,19 @@
     <t>Clean Profit</t>
   </si>
   <si>
+    <t>4780022250220</t>
+  </si>
+  <si>
     <t>Kurt Ermak</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>3000</t>
   </si>
   <si>
     <t>WL0047968</t>
@@ -77,10 +89,16 @@
     <t>Harry Potter</t>
   </si>
   <si>
-    <t>Kotta Non</t>
+    <t>20</t>
   </si>
   <si>
-    <t>12</t>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>Kotta Non</t>
   </si>
 </sst>
 </file>
@@ -147,28 +165,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,29 +484,30 @@
   <dimension ref="A1:L300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -511,19 +522,19 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1"/>
@@ -532,92 +543,89 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>4780022250220</v>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3">
-        <v>66</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E2" s="3">
         <v>100</v>
       </c>
       <c r="F2" s="3">
         <f>D2-E2</f>
-        <v>-34</v>
-      </c>
-      <c r="G2" s="4">
-        <v>2500</v>
-      </c>
-      <c r="H2" s="4">
-        <v>3000</v>
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I2" s="4">
-        <f>H2*E2</f>
+        <f t="shared" ref="I2:I26" si="0">H2*E2</f>
         <v>300000</v>
       </c>
-      <c r="J2" s="2">
-        <f>D2*G2</f>
-        <v>165000</v>
-      </c>
-      <c r="K2" s="2">
-        <f>I2-J2</f>
-        <v>135000</v>
+      <c r="J2" s="4">
+        <f t="shared" ref="J2:J26" si="1">D2*G2</f>
+        <v>250000</v>
+      </c>
+      <c r="K2" s="4">
+        <f t="shared" ref="K2:K26" si="2">I2-J2</f>
+        <v>50000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="3">
         <v>5</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="4">
-        <v>20000</v>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="I3" s="4">
-        <f>H3*E3</f>
+        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="J3" s="2">
-        <f>D3*G3</f>
-        <v>100000</v>
-      </c>
-      <c r="K3" s="2">
-        <f>I3-J3</f>
-        <v>0</v>
+      <c r="J3" s="4">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
+      <c r="K3" s="4">
+        <f t="shared" si="2"/>
+        <v>-100000</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="3">
         <v>123</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3">
         <v>90</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
       <c r="G4" s="4">
         <v>3500</v>
       </c>
@@ -625,15 +633,15 @@
         <v>4000</v>
       </c>
       <c r="I4" s="4">
-        <f>H4*E4</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <f>D4*G4</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
         <v>315000</v>
       </c>
-      <c r="K4" s="2">
-        <f>I4-J4</f>
+      <c r="K4" s="4">
+        <f t="shared" si="2"/>
         <v>-315000</v>
       </c>
     </row>
@@ -641,49 +649,36 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:I26" si="0">H5*E5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <f t="shared" ref="J5:J26" si="1">D5*G5</f>
-        <v>144</v>
-      </c>
-      <c r="K5" s="2">
-        <f t="shared" ref="K5:K26" si="2">I5-J5</f>
-        <v>-144</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -692,22 +687,15 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
       <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -716,22 +704,15 @@
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
       <c r="I8" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -740,22 +721,15 @@
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
       <c r="I9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -764,22 +738,15 @@
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -788,22 +755,15 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
       <c r="I11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -816,11 +776,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -833,11 +793,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -850,11 +810,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -867,11 +827,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -884,11 +844,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -901,11 +861,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -918,11 +878,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -935,11 +895,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -952,11 +912,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -969,11 +929,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -986,11 +946,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1003,11 +963,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1020,11 +980,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1037,11 +997,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1054,11 +1014,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
little improvement of inventory tab #2
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMS\Desktop\www\Python\Al_Halal_POS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B1A0A9-B5C0-4546-BA63-62117CEF0D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75D736A-F6D1-4AA7-A2A2-87D815D93796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>No</t>
   </si>
@@ -74,15 +74,6 @@
     <t>Kurt Ermak</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
     <t>WL0047968</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
   </si>
   <si>
     <t>20</t>
-  </si>
-  <si>
-    <t>10000</t>
   </si>
   <si>
     <t>20000</t>
@@ -105,10 +93,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$₩-412]* #,##0.00_-;\-[$₩-412]* #,##0.00_-;_-[$₩-412]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +107,17 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -162,10 +162,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,8 +180,24 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,8 +512,8 @@
     <col min="4" max="4" width="22.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="17" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" style="8" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" style="4" customWidth="1"/>
     <col min="10" max="10" width="17.44140625" style="4" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" style="4" customWidth="1"/>
@@ -522,10 +539,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -543,14 +560,14 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
+      <c r="D2" s="5">
+        <v>100</v>
       </c>
       <c r="E2" s="3">
         <v>100</v>
@@ -559,11 +576,11 @@
         <f>D2-E2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
+      <c r="G2" s="9">
+        <v>2500</v>
+      </c>
+      <c r="H2" s="9">
+        <v>3000</v>
       </c>
       <c r="I2" s="4">
         <f t="shared" ref="I2:I26" si="0">H2*E2</f>
@@ -583,22 +600,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>20</v>
+      <c r="G3" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" si="0"/>
@@ -621,15 +638,15 @@
         <v>123</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>90</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="8">
         <v>3500</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="8">
         <v>4000</v>
       </c>
       <c r="I4" s="4">
@@ -645,12 +662,15 @@
         <v>-315000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -668,8 +688,11 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
sell button design change
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="D2" s="5" t="n">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>100</v>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="D4" s="5" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>3500</v>

</xml_diff>

<commit_message>
button requires to fill barcode input now
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="D2" s="5" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>100</v>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="D4" s="5" t="n">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>3500</v>

</xml_diff>

<commit_message>
added + - buttons
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="D2" s="5" t="n">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>100</v>
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>5</v>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="D4" s="5" t="n">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>3500</v>

</xml_diff>

<commit_message>
refresh button, design changes
</commit_message>
<xml_diff>
--- a/data/POS_2025_03.xlsx
+++ b/data/POS_2025_03.xlsx
@@ -482,7 +482,7 @@
   <dimension ref="A1:L300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="D2" s="5" t="n">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>100</v>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="D4" s="5" t="n">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>3500</v>

</xml_diff>